<commit_message>
Cleaned up code and updated read.me file
</commit_message>
<xml_diff>
--- a/books.xlsx
+++ b/books.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\VisualStudio\BookshopVue\BookshopVue\assets\datasource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\VisualStudio\ExcelToJSON\ExcelToJSON\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF9FFDD-5CB4-4FAC-ADC8-3927D9759092}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA6312C-BED9-46C8-B291-655357D6DDB2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7455" yWindow="825" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="books" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="66">
   <si>
     <t>Title</t>
   </si>
@@ -64,6 +64,165 @@
   </si>
   <si>
     <t>Emperor of Thorns</t>
+  </si>
+  <si>
+    <t>The Sisters Brothers</t>
+  </si>
+  <si>
+    <t>Patrick DeWitt</t>
+  </si>
+  <si>
+    <t>The Essex Serpent</t>
+  </si>
+  <si>
+    <t>Western;Literature;Historical</t>
+  </si>
+  <si>
+    <t>Literature;Historical</t>
+  </si>
+  <si>
+    <t>Why I’m No Longer Talking to White People About Race</t>
+  </si>
+  <si>
+    <t>Reni Eddo-Lodge</t>
+  </si>
+  <si>
+    <t>Non-Fiction;Social Sciences</t>
+  </si>
+  <si>
+    <t>Sarah Perry</t>
+  </si>
+  <si>
+    <t>Cujo</t>
+  </si>
+  <si>
+    <t>Stephen King</t>
+  </si>
+  <si>
+    <t>Horror</t>
+  </si>
+  <si>
+    <t>Blackbirds</t>
+  </si>
+  <si>
+    <t>Chuck Wendig</t>
+  </si>
+  <si>
+    <t>Horror; Thriller</t>
+  </si>
+  <si>
+    <t>Hollow Things</t>
+  </si>
+  <si>
+    <t>T.S. King</t>
+  </si>
+  <si>
+    <t>Heart Shaped Box</t>
+  </si>
+  <si>
+    <t>Joe Hill</t>
+  </si>
+  <si>
+    <t>Buddha Da</t>
+  </si>
+  <si>
+    <t>Anne Donovan</t>
+  </si>
+  <si>
+    <t>Trainspotting</t>
+  </si>
+  <si>
+    <t>Irvine Welsh</t>
+  </si>
+  <si>
+    <t>The Crow Road</t>
+  </si>
+  <si>
+    <t>Iain Banks</t>
+  </si>
+  <si>
+    <t>Literature; Scottish</t>
+  </si>
+  <si>
+    <t>Klara and the Sun</t>
+  </si>
+  <si>
+    <t>Kazuo Ishiguro</t>
+  </si>
+  <si>
+    <t>Literature</t>
+  </si>
+  <si>
+    <t>One: Pot, Pan, Planet</t>
+  </si>
+  <si>
+    <t>Anna Jones</t>
+  </si>
+  <si>
+    <t>Non-Fiction;Cookery</t>
+  </si>
+  <si>
+    <t>The Midnight Library</t>
+  </si>
+  <si>
+    <t>Matt Haig</t>
+  </si>
+  <si>
+    <t>Modern Fiction</t>
+  </si>
+  <si>
+    <t>Acts of Desperation</t>
+  </si>
+  <si>
+    <t>Megan Nolan</t>
+  </si>
+  <si>
+    <t>Transcendant Kingdom</t>
+  </si>
+  <si>
+    <t>Yaa Gyasi</t>
+  </si>
+  <si>
+    <t>Difficult Women</t>
+  </si>
+  <si>
+    <t>Helen Lewis</t>
+  </si>
+  <si>
+    <t>Social Sciences</t>
+  </si>
+  <si>
+    <t>With These Hands</t>
+  </si>
+  <si>
+    <t>Pam Ayres</t>
+  </si>
+  <si>
+    <t>Biography</t>
+  </si>
+  <si>
+    <t>Empireland</t>
+  </si>
+  <si>
+    <t>Sathnam Sanghera</t>
+  </si>
+  <si>
+    <t>History; British History</t>
+  </si>
+  <si>
+    <t>The Thursday Murder Club</t>
+  </si>
+  <si>
+    <t>Richard Osman</t>
+  </si>
+  <si>
+    <t>Modern Fiction; Crime; Thriller</t>
+  </si>
+  <si>
+    <t>Luster</t>
+  </si>
+  <si>
+    <t>Raven Leilani</t>
   </si>
 </sst>
 </file>
@@ -390,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,6 +646,286 @@
         <v>8.99</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26">
+        <v>8.99</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Cleaned up code and updated read.me file (#3)
Co-authored-by: = <=>
</commit_message>
<xml_diff>
--- a/books.xlsx
+++ b/books.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\VisualStudio\BookshopVue\BookshopVue\assets\datasource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\VisualStudio\ExcelToJSON\ExcelToJSON\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF9FFDD-5CB4-4FAC-ADC8-3927D9759092}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA6312C-BED9-46C8-B291-655357D6DDB2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7455" yWindow="825" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="books" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="66">
   <si>
     <t>Title</t>
   </si>
@@ -64,6 +64,165 @@
   </si>
   <si>
     <t>Emperor of Thorns</t>
+  </si>
+  <si>
+    <t>The Sisters Brothers</t>
+  </si>
+  <si>
+    <t>Patrick DeWitt</t>
+  </si>
+  <si>
+    <t>The Essex Serpent</t>
+  </si>
+  <si>
+    <t>Western;Literature;Historical</t>
+  </si>
+  <si>
+    <t>Literature;Historical</t>
+  </si>
+  <si>
+    <t>Why I’m No Longer Talking to White People About Race</t>
+  </si>
+  <si>
+    <t>Reni Eddo-Lodge</t>
+  </si>
+  <si>
+    <t>Non-Fiction;Social Sciences</t>
+  </si>
+  <si>
+    <t>Sarah Perry</t>
+  </si>
+  <si>
+    <t>Cujo</t>
+  </si>
+  <si>
+    <t>Stephen King</t>
+  </si>
+  <si>
+    <t>Horror</t>
+  </si>
+  <si>
+    <t>Blackbirds</t>
+  </si>
+  <si>
+    <t>Chuck Wendig</t>
+  </si>
+  <si>
+    <t>Horror; Thriller</t>
+  </si>
+  <si>
+    <t>Hollow Things</t>
+  </si>
+  <si>
+    <t>T.S. King</t>
+  </si>
+  <si>
+    <t>Heart Shaped Box</t>
+  </si>
+  <si>
+    <t>Joe Hill</t>
+  </si>
+  <si>
+    <t>Buddha Da</t>
+  </si>
+  <si>
+    <t>Anne Donovan</t>
+  </si>
+  <si>
+    <t>Trainspotting</t>
+  </si>
+  <si>
+    <t>Irvine Welsh</t>
+  </si>
+  <si>
+    <t>The Crow Road</t>
+  </si>
+  <si>
+    <t>Iain Banks</t>
+  </si>
+  <si>
+    <t>Literature; Scottish</t>
+  </si>
+  <si>
+    <t>Klara and the Sun</t>
+  </si>
+  <si>
+    <t>Kazuo Ishiguro</t>
+  </si>
+  <si>
+    <t>Literature</t>
+  </si>
+  <si>
+    <t>One: Pot, Pan, Planet</t>
+  </si>
+  <si>
+    <t>Anna Jones</t>
+  </si>
+  <si>
+    <t>Non-Fiction;Cookery</t>
+  </si>
+  <si>
+    <t>The Midnight Library</t>
+  </si>
+  <si>
+    <t>Matt Haig</t>
+  </si>
+  <si>
+    <t>Modern Fiction</t>
+  </si>
+  <si>
+    <t>Acts of Desperation</t>
+  </si>
+  <si>
+    <t>Megan Nolan</t>
+  </si>
+  <si>
+    <t>Transcendant Kingdom</t>
+  </si>
+  <si>
+    <t>Yaa Gyasi</t>
+  </si>
+  <si>
+    <t>Difficult Women</t>
+  </si>
+  <si>
+    <t>Helen Lewis</t>
+  </si>
+  <si>
+    <t>Social Sciences</t>
+  </si>
+  <si>
+    <t>With These Hands</t>
+  </si>
+  <si>
+    <t>Pam Ayres</t>
+  </si>
+  <si>
+    <t>Biography</t>
+  </si>
+  <si>
+    <t>Empireland</t>
+  </si>
+  <si>
+    <t>Sathnam Sanghera</t>
+  </si>
+  <si>
+    <t>History; British History</t>
+  </si>
+  <si>
+    <t>The Thursday Murder Club</t>
+  </si>
+  <si>
+    <t>Richard Osman</t>
+  </si>
+  <si>
+    <t>Modern Fiction; Crime; Thriller</t>
+  </si>
+  <si>
+    <t>Luster</t>
+  </si>
+  <si>
+    <t>Raven Leilani</t>
   </si>
 </sst>
 </file>
@@ -390,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,6 +646,286 @@
         <v>8.99</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26">
+        <v>8.99</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>